<commit_message>
updated comments and finalised schedule.py
</commit_message>
<xml_diff>
--- a/outputs/logs/resultsAll.xlsx
+++ b/outputs/logs/resultsAll.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benedict\cs_projects\fyp\ferryServiceVRP\outputs\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E694E540-8871-44CB-90FC-C3C0E7654CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3A20E5-01FC-480A-A66B-0F93B304B157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{2233DD1C-34DB-4472-8459-636426A89A29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2233DD1C-34DB-4472-8459-636426A89A29}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Programming Model" sheetId="3" r:id="rId1"/>
     <sheet name="Genetic Algorithm" sheetId="4" r:id="rId2"/>
     <sheet name="Comparison" sheetId="1" r:id="rId3"/>
     <sheet name="Data Analysis" sheetId="5" r:id="rId4"/>
-    <sheet name="Archive" sheetId="6" r:id="rId5"/>
+    <sheet name="Archive" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="81">
   <si>
     <t>LT1</t>
   </si>
@@ -297,6 +297,15 @@
   <si>
     <t>Comparing the optimality, GA seems to perform less poorly on clustered datasets, one possible reason is that such problelms are generally less complex.</t>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Average fleetsize used</t>
+  </si>
+  <si>
+    <t>Average Tour Duration</t>
+  </si>
 </sst>
 </file>
 
@@ -370,7 +379,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -495,11 +504,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -584,6 +679,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9873,42 +9978,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22353FE8-9054-42AB-908E-E46762EEA4B1}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="50.28515625" customWidth="1"/>
-    <col min="25" max="25" width="58.5703125" customWidth="1"/>
-    <col min="26" max="26" width="80.42578125" customWidth="1"/>
-    <col min="27" max="27" width="11.85546875" customWidth="1"/>
-    <col min="28" max="28" width="55.140625" customWidth="1"/>
-    <col min="29" max="29" width="52.28515625" customWidth="1"/>
-    <col min="30" max="30" width="33.28515625" customWidth="1"/>
+    <col min="22" max="22" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="50.33203125" customWidth="1"/>
+    <col min="25" max="25" width="58.5546875" customWidth="1"/>
+    <col min="26" max="26" width="80.44140625" customWidth="1"/>
+    <col min="27" max="27" width="11.88671875" customWidth="1"/>
+    <col min="28" max="28" width="55.109375" customWidth="1"/>
+    <col min="29" max="29" width="52.33203125" customWidth="1"/>
+    <col min="30" max="30" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -9951,7 +10054,7 @@
       <c r="V1" s="22"/>
       <c r="X1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -10019,7 +10122,7 @@
       <c r="AC2" s="45"/>
       <c r="AD2" s="45"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
@@ -10079,7 +10182,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>1</v>
       </c>
@@ -10138,7 +10241,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
@@ -10197,7 +10300,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>3</v>
       </c>
@@ -10256,7 +10359,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>4</v>
       </c>
@@ -10315,7 +10418,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>5</v>
       </c>
@@ -10374,7 +10477,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
@@ -10433,7 +10536,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>6</v>
       </c>
@@ -10492,7 +10595,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>8</v>
       </c>
@@ -10551,7 +10654,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>9</v>
       </c>
@@ -10610,7 +10713,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>10</v>
       </c>
@@ -10669,7 +10772,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>11</v>
       </c>
@@ -10728,7 +10831,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>71</v>
       </c>
@@ -10787,7 +10890,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>72</v>
       </c>
@@ -10846,7 +10949,7 @@
         <v>29.96</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>73</v>
       </c>
@@ -10905,7 +11008,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="34" t="s">
         <v>74</v>
       </c>
@@ -10964,7 +11067,7 @@
         <v>135.85</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>28</v>
       </c>
@@ -11023,7 +11126,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>29</v>
       </c>
@@ -11082,7 +11185,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>30</v>
       </c>
@@ -11141,7 +11244,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
         <v>31</v>
       </c>
@@ -11200,7 +11303,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
         <v>32</v>
       </c>
@@ -11260,7 +11363,7 @@
       </c>
       <c r="Y23" s="68"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
         <v>33</v>
       </c>
@@ -11321,7 +11424,7 @@
       <c r="X24" s="68"/>
       <c r="Y24" s="68"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
         <v>34</v>
       </c>
@@ -11381,7 +11484,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>35</v>
       </c>
@@ -11440,7 +11543,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
         <v>36</v>
       </c>
@@ -11499,7 +11602,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>37</v>
       </c>
@@ -11558,7 +11661,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
         <v>38</v>
       </c>
@@ -11617,7 +11720,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
         <v>39</v>
       </c>
@@ -11677,7 +11780,7 @@
       </c>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
         <v>40</v>
       </c>
@@ -11737,41 +11840,41 @@
       </c>
       <c r="W31" s="3"/>
     </row>
-    <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35" t="s">
+    <row r="32" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="3">
         <v>122.6</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="3">
         <v>341</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="20">
         <v>463.6</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="3">
         <v>28</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="3">
         <v>0</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="21">
         <v>28</v>
       </c>
-      <c r="I32" s="35" t="s">
+      <c r="I32" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="J32" s="16">
+      <c r="J32" s="17">
         <v>5</v>
       </c>
-      <c r="K32" s="63">
+      <c r="K32" s="62">
         <v>2</v>
       </c>
-      <c r="L32" s="12">
+      <c r="L32" s="3">
         <v>5</v>
       </c>
-      <c r="M32" s="66">
+      <c r="M32" s="65">
         <v>2</v>
       </c>
       <c r="P32" s="35" t="s">
@@ -11797,17 +11900,86 @@
       </c>
       <c r="W32" s="3"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="84">
+        <f>AVERAGE(B3:B32)</f>
+        <v>108.15333333333328</v>
+      </c>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84">
+        <f>AVERAGE(E3:E32)</f>
+        <v>86.353333333333183</v>
+      </c>
+      <c r="F33" s="84"/>
+      <c r="G33" s="85"/>
+      <c r="I33" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" s="84">
+        <f>AVERAGE(J3:J32)</f>
+        <v>6.4666666666666668</v>
+      </c>
+      <c r="K33" s="84">
+        <f t="shared" ref="K33:M33" si="0">AVERAGE(K3:K32)</f>
+        <v>2.0666666666666669</v>
+      </c>
+      <c r="L33" s="84">
+        <f t="shared" si="0"/>
+        <v>6.4666666666666668</v>
+      </c>
+      <c r="M33" s="84">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="90" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="87"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87">
+        <f>(B33+E33)/2</f>
+        <v>97.253333333333231</v>
+      </c>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="88"/>
+      <c r="I34" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3">
+        <f>J33/K33</f>
+        <v>3.129032258064516</v>
+      </c>
+      <c r="L34" s="3"/>
+      <c r="M34" s="86">
+        <f>L33/M33</f>
+        <v>2.9846153846153847</v>
+      </c>
       <c r="W34" s="3"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="I35" s="90" t="s">
+        <v>79</v>
+      </c>
+      <c r="J35" s="87"/>
+      <c r="K35" s="87"/>
+      <c r="L35" s="87">
+        <f>(K34+M34)/2</f>
+        <v>3.0568238213399503</v>
+      </c>
+      <c r="M35" s="88"/>
       <c r="W35" s="3"/>
     </row>
-    <row r="39" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
@@ -11816,7 +11988,7 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
@@ -11825,7 +11997,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
@@ -11834,7 +12006,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
@@ -11843,7 +12015,7 @@
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
@@ -11852,7 +12024,7 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
@@ -11861,7 +12033,7 @@
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q46" s="3"/>
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
@@ -11871,11 +12043,11 @@
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="45"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -11893,7 +12065,7 @@
       <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="45"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -11911,7 +12083,7 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="45"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -11929,7 +12101,7 @@
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="45"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -11947,7 +12119,7 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="45"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -11963,7 +12135,7 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="45"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -11979,7 +12151,7 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="45"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -11995,7 +12167,7 @@
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="45"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -12011,7 +12183,7 @@
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="45"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -12027,7 +12199,7 @@
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="45"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -12043,7 +12215,7 @@
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="45"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -12059,7 +12231,7 @@
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="45"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -12075,7 +12247,7 @@
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -12091,7 +12263,7 @@
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -12107,7 +12279,7 @@
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -12126,6 +12298,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12133,19 +12306,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7A6337-75B7-43DD-A58F-79890A9B5199}">
   <dimension ref="A1:W87"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -12185,7 +12358,7 @@
       <c r="T1" s="5"/>
       <c r="U1" s="22"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -12245,7 +12418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
@@ -12305,7 +12478,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>1</v>
       </c>
@@ -12364,7 +12537,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
@@ -12423,7 +12596,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>3</v>
       </c>
@@ -12482,7 +12655,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>4</v>
       </c>
@@ -12541,7 +12714,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>5</v>
       </c>
@@ -12600,7 +12773,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>7</v>
       </c>
@@ -12659,7 +12832,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>6</v>
       </c>
@@ -12718,7 +12891,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>8</v>
       </c>
@@ -12777,7 +12950,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>9</v>
       </c>
@@ -12836,7 +13009,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>10</v>
       </c>
@@ -12895,7 +13068,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>11</v>
       </c>
@@ -12954,7 +13127,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>71</v>
       </c>
@@ -13013,7 +13186,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>72</v>
       </c>
@@ -13072,7 +13245,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>73</v>
       </c>
@@ -13131,7 +13304,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="35" t="s">
         <v>74</v>
       </c>
@@ -13190,7 +13363,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="33" t="s">
         <v>28</v>
       </c>
@@ -13249,7 +13422,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>29</v>
       </c>
@@ -13308,7 +13481,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>30</v>
       </c>
@@ -13367,7 +13540,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
         <v>31</v>
       </c>
@@ -13427,7 +13600,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
         <v>32</v>
       </c>
@@ -13487,7 +13660,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
         <v>33</v>
       </c>
@@ -13549,7 +13722,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
         <v>34</v>
       </c>
@@ -13611,7 +13784,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>35</v>
       </c>
@@ -13673,7 +13846,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
         <v>36</v>
       </c>
@@ -13735,7 +13908,7 @@
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>37</v>
       </c>
@@ -13797,7 +13970,7 @@
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
         <v>38</v>
       </c>
@@ -13859,7 +14032,7 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
         <v>39</v>
       </c>
@@ -13921,7 +14094,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
         <v>40</v>
       </c>
@@ -13983,7 +14156,7 @@
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="35" t="s">
         <v>41</v>
       </c>
@@ -14045,31 +14218,31 @@
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
     </row>
-    <row r="33" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:23" x14ac:dyDescent="0.3">
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:23" x14ac:dyDescent="0.3">
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
     </row>
-    <row r="35" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:23" x14ac:dyDescent="0.3">
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
     </row>
-    <row r="36" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:23" x14ac:dyDescent="0.3">
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
     </row>
-    <row r="37" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:23" x14ac:dyDescent="0.3">
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
     </row>
-    <row r="38" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="12:23" x14ac:dyDescent="0.3">
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
     </row>
-    <row r="39" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="12:23" x14ac:dyDescent="0.3">
       <c r="N39" s="3"/>
       <c r="O39" s="45"/>
       <c r="P39" s="3"/>
@@ -14081,7 +14254,7 @@
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
     </row>
-    <row r="40" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="12:23" x14ac:dyDescent="0.3">
       <c r="N40" s="3"/>
       <c r="O40" s="45"/>
       <c r="P40" s="3"/>
@@ -14093,7 +14266,7 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="12:23" x14ac:dyDescent="0.3">
       <c r="N41" s="3"/>
       <c r="O41" s="45"/>
       <c r="P41" s="3"/>
@@ -14105,7 +14278,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -14119,7 +14292,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -14133,7 +14306,7 @@
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
     </row>
-    <row r="44" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -14147,7 +14320,7 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
-    <row r="45" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -14161,7 +14334,7 @@
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
     </row>
-    <row r="46" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -14175,7 +14348,7 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
     </row>
-    <row r="47" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -14189,7 +14362,7 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="12:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -14203,143 +14376,143 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
     </row>
   </sheetData>
@@ -14353,33 +14526,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178B82E0-06C7-45F0-A54E-288505D84825}">
   <dimension ref="A1:Y90"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
+    <col min="17" max="17" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>13</v>
@@ -14400,7 +14573,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="22"/>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
@@ -14427,7 +14600,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="10"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>14</v>
       </c>
@@ -14477,7 +14650,7 @@
       <c r="W3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
@@ -14538,7 +14711,7 @@
         <v>-3.1546996684485142</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>1</v>
       </c>
@@ -14599,7 +14772,7 @@
         <v>4.9689440993778495</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>2</v>
       </c>
@@ -14660,7 +14833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>3</v>
       </c>
@@ -14721,7 +14894,7 @@
         <v>9.538950715421489</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>4</v>
       </c>
@@ -14782,7 +14955,7 @@
         <v>-0.25340933014199418</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>5</v>
       </c>
@@ -14843,7 +15016,7 @@
         <v>38.294741442841193</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>7</v>
       </c>
@@ -14904,7 +15077,7 @@
         <v>-1.6897821727982081</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>6</v>
       </c>
@@ -14965,7 +15138,7 @@
         <v>5.8902132443322177</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>8</v>
       </c>
@@ -15025,7 +15198,7 @@
         <v>265.3362783242149</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>9</v>
       </c>
@@ -15085,7 +15258,7 @@
         <v>120.19265520407774</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>10</v>
       </c>
@@ -15145,7 +15318,7 @@
         <v>238.67715024631337</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>11</v>
       </c>
@@ -15205,7 +15378,7 @@
         <v>513.75844584839683</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>71</v>
       </c>
@@ -15264,7 +15437,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
         <v>72</v>
       </c>
@@ -15323,7 +15496,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="31" t="s">
         <v>73</v>
       </c>
@@ -15382,7 +15555,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
         <v>74</v>
       </c>
@@ -15441,7 +15614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>28</v>
       </c>
@@ -15500,7 +15673,7 @@
         <v>52.75791646345791</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>29</v>
       </c>
@@ -15559,7 +15732,7 @@
         <v>63.620450769658476</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
         <v>30</v>
       </c>
@@ -15618,7 +15791,7 @@
         <v>15.497813099743382</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
         <v>31</v>
       </c>
@@ -15677,7 +15850,7 @@
         <v>-0.89043548698105346</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
         <v>32</v>
       </c>
@@ -15736,7 +15909,7 @@
         <v>15.540540540540546</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="34" t="s">
         <v>33</v>
       </c>
@@ -15795,7 +15968,7 @@
         <v>29.584580601972799</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>34</v>
       </c>
@@ -15854,7 +16027,7 @@
         <v>24.782290951360249</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
         <v>35</v>
       </c>
@@ -15913,7 +16086,7 @@
         <v>67.585676410520207</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
         <v>36</v>
       </c>
@@ -15972,7 +16145,7 @@
         <v>-2.2361641794387315</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="34" t="s">
         <v>37</v>
       </c>
@@ -16031,7 +16204,7 @@
         <v>9.8118820109606446</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
         <v>38</v>
       </c>
@@ -16090,7 +16263,7 @@
         <v>-19.790232056746888</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
         <v>39</v>
       </c>
@@ -16149,7 +16322,7 @@
         <v>-0.43215456949067188</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="34" t="s">
         <v>40</v>
       </c>
@@ -16208,7 +16381,7 @@
         <v>4.5977011494252924</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="35" t="s">
         <v>41</v>
       </c>
@@ -16269,8 +16442,8 @@
         <v>-8.244369021907147</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>13</v>
@@ -16298,7 +16471,7 @@
       <c r="R35" s="6"/>
       <c r="S35" s="7"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>26</v>
       </c>
@@ -16338,7 +16511,7 @@
       </c>
       <c r="S36" s="10"/>
     </row>
-    <row r="37" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>14</v>
       </c>
@@ -16390,7 +16563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="30" t="s">
         <v>0</v>
       </c>
@@ -16458,7 +16631,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>1</v>
       </c>
@@ -16526,7 +16699,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
         <v>2</v>
       </c>
@@ -16594,7 +16767,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>3</v>
       </c>
@@ -16662,7 +16835,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>4</v>
       </c>
@@ -16730,7 +16903,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>5</v>
       </c>
@@ -16798,7 +16971,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>7</v>
       </c>
@@ -16866,7 +17039,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>6</v>
       </c>
@@ -16934,7 +17107,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="31" t="s">
         <v>8</v>
       </c>
@@ -17002,7 +17175,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
         <v>9</v>
       </c>
@@ -17070,7 +17243,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
         <v>10</v>
       </c>
@@ -17138,7 +17311,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
         <v>11</v>
       </c>
@@ -17206,7 +17379,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="34" t="s">
         <v>71</v>
       </c>
@@ -17274,7 +17447,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="34" t="s">
         <v>72</v>
       </c>
@@ -17342,7 +17515,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="34" t="s">
         <v>73</v>
       </c>
@@ -17410,7 +17583,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="35" t="s">
         <v>74</v>
       </c>
@@ -17478,7 +17651,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="33" t="s">
         <v>28</v>
       </c>
@@ -17547,7 +17720,7 @@
       </c>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="34" t="s">
         <v>29</v>
       </c>
@@ -17616,7 +17789,7 @@
       </c>
       <c r="T55" s="3"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="34" t="s">
         <v>30</v>
       </c>
@@ -17685,7 +17858,7 @@
       </c>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="34" t="s">
         <v>31</v>
       </c>
@@ -17754,7 +17927,7 @@
       </c>
       <c r="T57" s="3"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="34" t="s">
         <v>32</v>
       </c>
@@ -17823,7 +17996,7 @@
       </c>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="34" t="s">
         <v>33</v>
       </c>
@@ -17891,7 +18064,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="34" t="s">
         <v>34</v>
       </c>
@@ -17959,7 +18132,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="34" t="s">
         <v>35</v>
       </c>
@@ -18027,7 +18200,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="34" t="s">
         <v>36</v>
       </c>
@@ -18095,7 +18268,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="34" t="s">
         <v>37</v>
       </c>
@@ -18163,7 +18336,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="34" t="s">
         <v>38</v>
       </c>
@@ -18231,7 +18404,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="34" t="s">
         <v>39</v>
       </c>
@@ -18299,7 +18472,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="34" t="s">
         <v>40</v>
       </c>
@@ -18367,7 +18540,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="35" t="s">
         <v>41</v>
       </c>
@@ -18435,35 +18608,35 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="82" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L83" s="3"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L84" s="3"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
     </row>
-    <row r="85" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="12:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L90" s="3"/>
     </row>
   </sheetData>
@@ -18477,17 +18650,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="82" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
@@ -18501,21 +18674,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63E007A-B4F4-42D1-B999-C7560A275CB5}">
   <dimension ref="A3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="88.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="87.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -18532,8 +18705,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="82" t="s">
         <v>44</v>
       </c>
       <c r="B5" t="s">
@@ -18543,8 +18716,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="82" t="s">
         <v>45</v>
       </c>
       <c r="B6" t="s">
@@ -18554,7 +18727,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -18568,7 +18741,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -18582,7 +18755,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -18596,7 +18769,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -18610,7 +18783,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -18624,8 +18797,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="82" t="s">
         <v>50</v>
       </c>
       <c r="B18" t="s">
@@ -18635,8 +18808,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="82" t="s">
         <v>49</v>
       </c>
       <c r="B19" t="s">
@@ -18646,7 +18819,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="83"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>76</v>
       </c>
@@ -18656,27 +18832,27 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="45" t="s">
         <v>61</v>
       </c>

</xml_diff>